<commit_message>
test: fixed test data
</commit_message>
<xml_diff>
--- a/app/_test_files/student-data.xlsx
+++ b/app/_test_files/student-data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>Origin Name</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Canvas ID</t>
+  </si>
+  <si>
+    <t>Image Vector512</t>
   </si>
   <si>
     <t>Байден Джо Байденович</t>
@@ -93,6 +96,9 @@
     <t>F99900221</t>
   </si>
   <si>
+    <t>[1.3962409496307373, 0.25348520278930664, 0.12064001709222794, 2.0256197452545166, 2.0230019092559814, 0.20399579405784607, -1.1738635301589966, 0.6804453730583191, 1.2862316370010376, 0.17690835893154144, 1.0834029912948608, 1.7227295637130737, 0.36781683564186096, 0.9594988822937012, -0.647626519203186, -0.34818366169929504, 0.6643533110618591, 0.9534273147583008, -1.6178522109985352, 1.4374622106552124, -1.0059338808059692, 0.3460935950279236, 0.15563449263572693, -2.0972185134887695, -1.799588918685913, 0.42877376079559326, 0.8938292860984802, 0.6677727699279785, -0.11484827101230621, 0.6909616589546204, 0.15080159902572632, -0.22230419516563416, -0.04757406562566757, 0.12934228777885437, -0.8585926294326782, -1.1926199197769165, -1.2092405557632446, -1.1465041637420654, -1.793269157409668, 1.043143630027771, -0.9808752536773682, -0.07618039101362228, 0.3461223840713501, -0.1563025265932083, -0.4514497220516205, 0.7905265092849731, 0.9158525466918945, 1.3487859964370728, -1.183567762374878, -1.1409316062927246, 0.04436982423067093, -1.464025616645813, 1.7240198850631714, 0.9445248246192932, -0.3032023310661316, -0.4634922444820404, -0.8888739943504333, 0.406692236661911, -0.06230883672833443, -0.5453231334686279, -0.2833837866783142, 0.15739253163337708, -0.5349299907684326, 0.5328725576400757, -0.7626968622207642, 0.5848228931427002, -0.4614882171154022, -1.159769892692566, 1.591030478477478, -0.393146812915802, 0.30914923548698425, 0.10887198150157928, -0.18616826832294464, -0.42824631929397583, -0.4392251968383789, -0.7417682409286499, -0.12130074203014374, -1.6738035678863525, 0.1583893895149231, 0.7789269685745239, 0.8325433135032654, 0.3412347733974457, 1.0795903205871582, -0.35461127758026123, 0.018243849277496338, 0.4507361948490143, -0.047212183475494385, -1.109826922416687, -0.2842399775981903, -0.3438129425048828, 0.050584640353918076, 0.8657655119895935, 1.62526273727417, -1.3798843622207642, 0.776328444480896, 1.958412528038025, 0.5927445292472839, 1.8461605310440063, 0.15654027462005615, 0.13759522140026093, -0.250734806060791, 1.8075417280197144, 0.3351730704307556, 1.6057838201522827, 0.9526150822639465, 0.3634589910507202, 0.5026417374610901, -0.40205812454223633, 0.0023490963503718376, 0.15849249064922333, 1.0077459812164307, -0.19005624949932098, -1.3875013589859009, -0.70941561460495, -0.0730259045958519, 0.039034586399793625, 1.252573847770691, 0.32731208205223083, -0.0011512786149978638, -0.25025251507759094, 0.0014034248888492584, 1.4484443664550781, -1.0040948390960693, -2.09417462348938, -0.32473376393318176, -2.2173092365264893, 0.4221401810646057, -2.011507272720337, -0.8740596175193787, -0.5818102359771729, -0.7911050915718079, 0.8592305779457092, 0.5408867597579956, -0.038635335862636566, -1.8204666376113892, -0.23744149506092072, -1.3665193319320679, -1.279675006866455, 1.8475995063781738, 1.7864826917648315, 1.541104793548584, 1.1277824640274048, -1.9106066226959229, 1.0935595035552979, 1.4984331130981445, 0.38109439611434937, -0.7003207206726074, -0.37998902797698975, -0.9380583167076111, 0.648933470249176, 1.2857705354690552, 0.10497797280550003, -1.5645326375961304, 3.081533670425415, 0.3812711834907532, -0.8002382516860962, -0.7335601449012756, -0.7562578916549683, -1.8197816610336304, -1.2430131435394287, 1.340442419052124, 1.6229056119918823, 0.4408093988895416, 0.6820831298828125, 0.3240942656993866, 0.6942362785339355, -0.2753414511680603, 0.07724416255950928, -1.3861411809921265, 1.0982407331466675, -0.49474185705184937, 1.0112475156784058, -0.13035275042057037, 0.9232515096664429, 1.740647792816162, 0.7432114481925964, -0.6233522295951843, -0.17351016402244568, -0.33036288619041443, 0.5222566723823547, -0.39664286375045776, 0.2605922818183899, -2.18696928024292, -0.6645631790161133, 1.3879423141479492, 0.8855301737785339, 0.12846991419792175, 0.5378470420837402, 2.155102014541626, 1.0465387105941772, 0.15678586065769196, 0.7731473445892334, 0.316240131855011, -1.3448196649551392, 0.9672431349754333, 1.0760198831558228, -0.05247711390256882, -0.07243874669075012, 0.7794440984725952, -1.3360745906829834, 1.5258311033248901, -0.9074477553367615, 0.16537047922611237, -0.22329874336719513, 1.3353098630905151, 1.0480793714523315, 0.6799889206886292, 0.44181787967681885, 0.29475364089012146, 1.2851070165634155, -0.8851805925369263, -0.7460017800331116, 0.8608453273773193, -0.11279578506946564, 0.732658326625824, 0.4515901207923889, -1.0451834201812744, 1.3582375049591064, -1.7141224145889282, -0.13853737711906433, -1.7189503908157349, -1.2173926830291748, 0.6103136539459229, -0.017051391303539276, 0.6633625626564026, 1.1715182065963745, 0.3767896294593811, 0.6686310172080994, 0.36128732562065125, 0.23263315856456757, 1.2081400156021118, -0.659639835357666, 0.08537419140338898, -1.9784958362579346, -0.980346143245697, -0.6622186303138733, -1.7514352798461914, 0.8565031290054321, 0.8315029144287109, 0.7265191078186035, 1.1494946479797363, 0.35799580812454224, 0.9063497185707092, -0.6682062149047852, 0.30700674653053284, 1.3203966617584229, 0.12042892724275589, -0.5198970437049866, -0.16074976325035095, 1.2513682842254639, -0.788196325302124, 0.7180217504501343, 1.7709152698516846, -0.08279925584793091, 1.1078159809112549, 1.1104110479354858, -0.352237731218338, 1.2850589752197266, 0.07303699851036072, 0.08361196517944336, -0.6342514157295227, 0.5712156891822815, 1.423522710800171, -1.9228776693344116, -0.11095533519983292, -0.8966971635818481, 0.12803152203559875, 1.205467700958252, -0.26026079058647156, -1.7507240772247314, 0.04638421908020973, 0.11738766729831696, 1.8209387063980103, -0.3024059236049652, 0.4740696847438812, 1.1813119649887085, 1.4482421875, 0.3587510585784912, 0.38016557693481445, 0.3809036910533905, 0.3683170676231384, 2.033905506134033, -1.472590446472168, 0.14776815474033356, -1.9124960899353027, -0.8451277613639832, -0.0444989949464798, 1.4864035844802856, -1.0731642246246338, 0.8196827173233032, -1.3446717262268066, -1.3022723197937012, -0.011484291404485703, 0.4653628468513489, 0.7271881699562073, -1.301723837852478, -1.0194069147109985, -0.8949748873710632, 0.12421716749668121, -1.3974156379699707, 0.874057412147522, -0.16972392797470093, -0.40540027618408203, -0.26660504937171936, -0.08859006315469742, 0.4087318181991577, -0.014617778360843658, -0.4927877187728882, -1.5463612079620361, 1.0609203577041626, -0.5740880370140076, 1.0580521821975708, 0.3201751112937927, 1.0859293937683105, 1.04197096824646, 0.8479683995246887, -1.0782862901687622, 1.345812439918518, 1.4105111360549927, 0.8742429614067078, 0.8079293966293335, 0.17397911846637726, 0.7060045003890991, 1.0472710132598877, -0.49078574776649475, -0.2443741261959076, -0.5875128507614136, 1.6156229972839355, -0.016354652121663094, -0.07448151707649231, 1.929330825805664, 0.7787438631057739, 0.40754181146621704, -0.19732484221458435, 0.040284134447574615, 0.8815439343452454, 0.8708389401435852, -0.9117416143417358, 0.18458186089992523, -0.5696215629577637, 1.077522873878479, 0.0739370808005333, -0.009541633538901806, -0.7774196863174438, 0.7028521299362183, -0.26334503293037415, -1.5373259782791138, 1.0169187784194946, 0.13380290567874908, -1.5972931385040283, -0.4724063575267792, -0.22362041473388672, 0.46148863434791565, -1.254451870918274, -0.1764441281557083, -0.2404455989599228, 0.7556658983230591, 0.5199664235115051, -0.008495435118675232, 1.3922802209854126, -0.7887707948684692, 0.3305409848690033, -0.1786080151796341, -0.13785763084888458, 0.032301969826221466, -0.6760828495025635, -1.7926478385925293, -0.08383653312921524, 1.0863834619522095, 0.06826242804527283, -0.732753574848175, -1.081466555595398, -0.30018913745880127, 0.17522934079170227, -0.45162779092788696, 2.396880865097046, -0.4635702967643738, 2.1411731243133545, -0.4805733263492584, 0.13686539232730865, -1.6508485078811646, -1.5408995151519775, -1.3572763204574585, -1.2039884328842163, -0.2857149839401245, -0.3561415672302246, 0.10026409476995468, 0.002783350646495819, 0.03674301505088806, -0.36973142623901367, -0.03957793861627579, 0.8505733013153076, -0.6826883554458618, 1.0721698999404907, -0.1274060755968094, 1.39711594581604, 1.1327061653137207, 1.1782143115997314, 2.015730142593384, -1.2300249338150024, -0.18113595247268677, 0.9700377583503723, 0.3764283061027527, 0.04577576369047165, 1.1069835424423218, 0.046110548079013824, -2.0855252742767334, -1.635956048965454, -0.4584546983242035, 0.42028242349624634, 0.8831629157066345, -0.56447434425354, 1.9608904123306274, -1.0740965604782104, 0.0683947503566742, 0.40688514709472656, 1.3164130449295044, 0.6535145044326782, 0.3487345576286316, -0.7572197318077087, 1.7863363027572632, 0.23929758369922638, 0.20364028215408325, 0.5648829340934753, -0.3979513347148895, 0.8923723697662354, -1.6784523725509644, 0.013624009676277637, 0.6801648139953613, -1.223663568496704, -0.8254892230033875, -0.012522481381893158, -0.9841986894607544, -0.4082798957824707, 0.7689269781112671, 0.15756827592849731, -1.5597620010375977, -0.8401668667793274, 0.16813203692436218, 0.28747543692588806, -1.2258154153823853, -0.08960852771997452, -1.0438703298568726, 2.147334575653076, -1.6981309652328491, 1.710310697555542, -0.9774251580238342, -1.7410802841186523, -0.355048269033432, -1.3362658023834229, -0.5879631042480469, -0.10362716764211655, -0.20228974521160126, 0.1199280172586441, 0.6447665691375732, 0.17291483283042908, -0.45042183995246887, -1.2204848527908325, 0.7485648393630981, -0.23133522272109985, 0.994961678981781, 0.3339676558971405, 0.061829790472984314, -0.4948424696922302, -0.44491755962371826, -0.5238187313079834, 0.4047211706638336, -1.4231657981872559, 0.1654396802186966, 0.34408536553382874, -0.07818707823753357, -0.6820454001426697, 0.6147446036338806, -0.6676418781280518, -1.1526025533676147, 1.2383496761322021, 1.0234899520874023, -0.9420217871665955, 1.0749763250350952, 0.7816265821456909, 0.3686220645904541, 2.084192991256714, -1.0175758600234985, -0.9284012913703918, -0.5218203663825989, -0.6600774526596069, -1.6440210342407227, 1.35569167137146, -0.508039116859436, -0.6610211133956909, -0.8103209733963013, -0.07767023146152496, -0.794180154800415, 0.3560171127319336, 0.9745310544967651, -0.8873608708381653, -0.22164782881736755, -0.19281010329723358, 0.5105790495872498, 0.3453094959259033, 0.22860082983970642, 0.22721539437770844, -1.0384107828140259, -2.2334091663360596, 0.0738895833492279, 1.0038725137710571, 0.5083069205284119, -0.7262762188911438, 0.751910924911499, -0.24997715651988983, 0.8769075870513916, 0.32690873742103577]</t>
+  </si>
+  <si>
     <t>Нурсултан Нурсултан Нурсултанович</t>
   </si>
   <si>
@@ -155,6 +161,9 @@
     <t>F17005999</t>
   </si>
   <si>
+    <t>[-0.7961677312850952, 0.9637256860733032, -1.001526951789856, 0.3349078595638275, 0.5341723561286926, -1.768042802810669, -0.16231946647167206, 1.6421688795089722, 0.8530632257461548, 0.3288135230541229, 1.843158483505249, 0.08279640972614288, 1.3436315059661865, 0.629977285861969, 0.4747724235057831, -1.07329261302948, -0.7958799600601196, -0.10003389418125153, -1.8091951608657837, 0.7989112138748169, -1.0585147142410278, -0.47361019253730774, 0.06997755169868469, -1.833152413368225, -0.61170893907547, -1.3900039196014404, 0.7683635950088501, -1.0562043190002441, 0.46653836965560913, -0.706555187702179, 0.275371253490448, 0.46728917956352234, -0.010401960462331772, 1.056440830230713, -0.3390531837940216, 0.13392187654972076, 0.19332730770111084, -0.1432792842388153, -0.5984602570533752, 0.07730454206466675, -1.3065979480743408, 0.41029468178749084, 1.0950846672058105, -0.4263962507247925, -0.5129979252815247, 0.8544540405273438, 1.260074496269226, 0.2968835234642029, -0.4247879385948181, -1.3823257684707642, -0.1927306354045868, -0.44728437066078186, 0.37659189105033875, -0.024884074926376343, -0.8135665655136108, -0.03828669339418411, -1.5834883451461792, -0.18442478775978088, -1.2569305896759033, -0.9658980965614319, -1.8618199825286865, 0.7068185806274414, -1.403983235359192, 0.7589347958564758, 0.31694892048835754, -1.0350415706634521, -1.2410694360733032, -0.6070502996444702, 1.2183034420013428, -0.4874742031097412, 0.22592520713806152, -0.4975467920303345, -0.6778320670127869, -1.255155086517334, 0.1393750011920929, -1.0231956243515015, -0.06367795169353485, -1.6800400018692017, -0.9132145643234253, 0.06476680934429169, 0.9291683435440063, 1.6437052488327026, 1.2123810052871704, -0.39149168133735657, 0.32127633690834045, 1.999769926071167, -0.23112687468528748, -0.5380033850669861, 0.5065725445747375, 0.7326056957244873, -0.5463383197784424, 1.3962833881378174, 0.0896141305565834, -2.0395700931549072, 0.23905891180038452, 1.5829038619995117, -0.4645441770553589, 0.6413150429725647, 0.32908040285110474, -1.6869014501571655, -0.41085147857666016, 1.7186411619186401, 1.023850917816162, 0.7571267485618591, -0.7701276540756226, 0.22452205419540405, -0.12191309034824371, -1.1212832927703857, -0.37788695096969604, -0.3367893099784851, 0.07756108045578003, 0.909173309803009, -0.13525578379631042, -0.09326633810997009, -0.8008986115455627, 1.292598009109497, 0.6243991255760193, 1.4427452087402344, -0.10779260098934174, 0.461859792470932, -0.7532594203948975, -0.5727448463439941, 0.6800729632377625, -0.8767865896224976, -0.23498520255088806, -1.2024537324905396, 0.2938215732574463, -0.9201697707176208, -1.2448878288269043, -1.7644919157028198, 0.5842075347900391, 1.555248498916626, 0.3458016812801361, 0.11687961220741272, 1.8784304857254028, 0.14628469944000244, -0.8253921270370483, -1.5933656692504883, -0.7400355339050293, 0.53778475522995, -0.9879505038261414, 1.9628280401229858, -1.4824104309082031, 0.8860349059104919, 0.7706769704818726, 1.3967068195343018, -0.9353098273277283, 1.6366796493530273, 0.379692018032074, 0.7902551293373108, 1.1294679641723633, -0.23239603638648987, -0.28733009099960327, 2.3431077003479004, -0.11362212896347046, 1.1928834915161133, 0.026152707636356354, -0.629342794418335, -0.08521448820829391, -2.138511896133423, 2.000643253326416, 1.562441110610962, 0.1292451024055481, -0.8603439331054688, 0.38861411809921265, -0.6798608899116516, -1.3369075059890747, -0.22621570527553558, -0.7547034621238708, 0.2726331949234009, -0.7062390446662903, 0.2938786447048187, -0.6932722330093384, 0.16932283341884613, -0.930834174156189, -0.04853210970759392, -0.3595499098300934, -1.1729216575622559, -0.6413623690605164, -0.36823296546936035, 1.1406241655349731, -0.5263634920120239, -0.21056734025478363, 0.5903757214546204, 0.8372596502304077, 1.576067328453064, 0.5142272710800171, 0.5352945327758789, 0.6180416941642761, 0.4037475883960724, -0.47864583134651184, 0.9808719158172607, -0.17868006229400635, -0.3554740846157074, 1.1546820402145386, 0.3199249804019928, 0.21229016780853271, -0.799119770526886, 0.758614182472229, 0.1825370490550995, -0.5845738053321838, -1.6706337928771973, 0.6042160987854004, -0.4164917767047882, 0.7908186316490173, 1.7419989109039307, 0.1122361421585083, -0.19340376555919647, 0.7330704927444458, 1.0522631406784058, -0.2648688554763794, 0.9721376299858093, -0.37228792905807495, -1.4151109457015991, -0.30410972237586975, -0.21984893083572388, -0.3439265489578247, 0.7119644284248352, 0.31239786744117737, -0.5312186479568481, 0.2979925870895386, 0.22587062418460846, 0.29331108927726746, 0.07629140466451645, 1.2575690746307373, 0.7199651598930359, 0.1903359740972519, 0.8172617554664612, -0.6437082290649414, -0.05871165916323662, -0.4906976521015167, -0.08893901854753494, 0.41995638608932495, 0.3819831907749176, -0.7572354078292847, -0.23358272016048431, -0.15369831025600433, -0.5882437825202942, 0.5967987775802612, 0.6575839519500732, 1.0032280683517456, 0.36386269330978394, -0.9182122945785522, -0.8716762065887451, -1.5980104207992554, 0.48119625449180603, -2.022080183029175, 0.37112554907798767, -0.39661750197410583, 1.2217158079147339, -0.7404541373252869, -0.015729423612356186, 0.8280972838401794, 0.28512459993362427, 0.09562388062477112, 0.3022276759147644, 0.8572600483894348, -0.1777392327785492, 1.0612484216690063, -1.1416232585906982, -0.08308620005846024, -1.0238831043243408, 1.055490493774414, -0.9827769994735718, 0.2966023087501526, -0.047581981867551804, -0.20893466472625732, 0.5223715901374817, 0.6871223449707031, -1.138199806213379, -0.18699757754802704, 0.08474798500537872, 0.8743605613708496, 0.10182323306798935, 0.3457656502723694, 0.664965033531189, -0.004542859736829996, 0.864875078201294, 0.36998727917671204, 1.664381742477417, -1.1508289575576782, 0.4283571243286133, 0.5142743587493896, -0.0688188225030899, -0.6515324115753174, -0.15247194468975067, 2.0300557613372803, 0.9532918930053711, -0.34357762336730957, -0.7649812698364258, 0.6336461305618286, -0.3156631290912628, -0.5003065466880798, 0.5981436967849731, -1.0441579818725586, -0.9076126217842102, 0.14674122631549835, -0.34567418694496155, 0.7474238872528076, 0.311644047498703, -0.6183782815933228, 1.0775165557861328, -1.294479489326477, -1.534759283065796, 1.6930640935897827, -1.2334048748016357, 0.3350287973880768, -0.18891143798828125, -1.029170274734497, 0.26004496216773987, -0.7459147572517395, 0.8377528190612793, -0.5773438811302185, -0.9738301634788513, 1.415360689163208, 0.11654160916805267, 0.6563736200332642, 0.7660938501358032, 1.099141240119934, 0.7713083028793335, -0.4515990614891052, -0.3698303699493408, 1.5370444059371948, 0.40919551253318787, 0.20602808892726898, -0.5480121970176697, 0.636358916759491, 1.5924066305160522, 1.6118592023849487, -0.1456080824136734, 0.8049397468566895, 0.530814528465271, 0.11072506755590439, 0.19788402318954468, -1.037956714630127, 0.6207442283630371, -0.28603535890579224, -0.46950748562812805, 0.7083088755607605, -0.022094953805208206, 1.2913259267807007, -0.30674079060554504, -1.6493451595306396, -0.1568288505077362, 1.7427870035171509, 0.23601539433002472, -0.6256807446479797, 1.071048378944397, 1.1914502382278442, 0.3010510206222534, 0.9198786020278931, -0.7980385422706604, 0.9678086638450623, -0.3409234583377838, 1.5902336835861206, -0.9511688351631165, -1.7283151149749756, 0.30660489201545715, -0.5640905499458313, 0.2161117047071457, 0.841410219669342, -1.6256972551345825, -1.620139241218567, -0.3325413465499878, 1.476622462272644, -1.0903500318527222, 0.567707359790802, 0.0381879098713398, 0.4961816966533661, -0.05972243472933769, -0.2647252380847931, -1.4830678701400757, 0.6597169041633606, -0.16314101219177246, -0.5909312963485718, 0.8109739422798157, 0.6226853132247925, 0.06095672398805618, -1.0814907550811768, 0.3593898415565491, -0.7982280850410461, -1.584344506263733, -0.10174717009067535, -1.3503365516662598, -1.1751190423965454, -0.40115413069725037, -0.5115169882774353, 1.2017642259597778, 1.1091487407684326, -0.5037769079208374, -1.3433420658111572, 0.745647132396698, -0.6284698843955994, 0.035480059683322906, 1.3081308603286743, 0.5228875875473022, 0.5432054400444031, 0.846739649772644, 0.8133434653282166, -0.7833893299102783, -0.302505224943161, -0.27957606315612793, 1.1324408054351807, 0.15402445197105408, 0.9224604368209839, 1.123585820198059, -0.5730285048484802, 1.175559163093567, -0.5464288592338562, -1.277226209640503, -0.25818711519241333, -0.6458134055137634, 0.6651991605758667, 0.3479243516921997, -1.4780195951461792, 1.1954216957092285, 0.8286364674568176, 1.0188051462173462, -1.549039363861084, 0.42931368947029114, 0.6960439085960388, 0.7617568969726562, -0.53224116563797, 1.2472996711730957, -0.7213504910469055, 0.920745313167572, -1.4783461093902588, -0.16380508244037628, 0.9658218622207642, -0.22484838962554932, -0.6910757422447205, -0.6132253408432007, 0.5478785037994385, 1.2923988103866577, 0.041623279452323914, -0.5550796985626221, -1.8026869297027588, -1.6971418857574463, -1.4308863878250122, -0.4180643856525421, -0.41918909549713135, -0.5600045323371887, 1.3371570110321045, 1.4045490026474, 0.7076674699783325, 1.5811498165130615, 0.3940381705760956, -0.7779830694198608, 0.4026751220226288, 0.44189703464508057, -0.8069300055503845, 0.8249001502990723, 1.825053334236145, -1.178694486618042, -0.014041949063539505, 1.511785626411438, 0.13227690756320953, 0.5042908787727356, 0.9081806540489197, -0.7216489911079407, 1.4931050539016724, 0.6011382937431335, 0.7584481835365295, -2.0803658962249756, -0.6968228220939636, -0.19259606301784515, 0.2908994257450104, 0.3209151029586792, -0.8669224977493286, 1.3177200555801392, -0.36617088317871094, 0.3581629991531372, -0.4667634963989258, 0.2251862734556198, 0.7419695258140564, 1.1182098388671875, -0.4409390091896057, -0.2819502353668213, 1.2876017093658447, 0.125426784157753, 0.9284355640411377, -0.139555424451828, -1.739342451095581, -0.9121516346931458, -0.5204627513885498, -0.41142868995666504, -0.32213884592056274, 1.2622685432434082, 0.3992549777030945, 0.3401094377040863, -0.16265128552913666, -1.4022390842437744, 0.33015701174736023, 1.0717610120773315, 0.7880427241325378, -1.7813206911087036, 0.5276214480400085, -0.3123737871646881, 1.2760593891143799, -0.8269984126091003, -0.6301215887069702, -1.6647639274597168, -0.7685734033584595, -0.5072072148323059, -0.6779585480690002, 1.2186846733093262, -0.7455694675445557, 0.021074488759040833, 1.892949104309082, -0.8763399720191956, 1.3087763786315918, 1.95158052444458]</t>
+  </si>
+  <si>
     <t>Токаев Касым Токаевич</t>
   </si>
   <si>
@@ -217,6 +226,9 @@
     <t>S23008808</t>
   </si>
   <si>
+    <t>[-0.8239181041717529, -0.10853372514247894, -1.090545415878296, -0.7254461050033569, 1.7563859224319458, 1.7485616207122803, 1.4564449787139893, 0.5298517346382141, -1.3817399740219116, 0.8451629281044006, -0.5875135660171509, -0.14625734090805054, -0.37666645646095276, 1.2832112312316895, -0.010950582101941109, -1.0970276594161987, -0.7279935479164124, 2.886953353881836, -1.1502999067306519, -0.037265751510858536, -0.3322172462940216, 1.869786024093628, 0.88702392578125, -0.27471667528152466, 0.08352775126695633, -0.39844322204589844, -0.686955451965332, -0.7674039006233215, 0.19696420431137085, -0.5749936699867249, 0.6078059077262878, 0.7594730854034424, 1.5007765293121338, 0.8598932027816772, 2.3760969638824463, 0.8672524094581604, 0.9394579529762268, -0.5731072425842285, 0.36647307872772217, -0.0003006681799888611, -0.06831717491149902, -0.5484591722488403, -0.16627900302410126, -0.6842096447944641, -0.8114863038063049, -0.6274036765098572, -0.9563456773757935, 0.22853541374206543, -0.9374585151672363, -0.12301567196846008, -1.9242208003997803, -1.8881604671478271, 0.8056733012199402, 1.488337755203247, -0.11040730774402618, -0.42356589436531067, -0.21843600273132324, 0.5700476169586182, 0.9641066193580627, -2.056166648864746, 0.6953127980232239, 2.2424538135528564, -0.07076992094516754, -0.9309090375900269, -0.5721548199653625, -1.8723102807998657, 0.850500762462616, -0.46838828921318054, 1.6810261011123657, 1.9760932922363281, -1.5297914743423462, -1.2943038940429688, -0.548575222492218, -0.49220073223114014, 0.837839663028717, 0.4648135006427765, 0.037809960544109344, 0.014784020371735096, -0.6184535026550293, -1.602264642715454, 0.4565237760543823, 0.8858281970024109, 0.6206457018852234, 0.0687495544552803, -0.02348882146179676, 0.6559999585151672, 0.5801131725311279, -0.8396305441856384, -1.799071192741394, -1.8141826391220093, 0.4337087571620941, 0.04646211862564087, 0.7730727791786194, -0.41511958837509155, 2.930788993835449, -0.03051912784576416, -1.0522352457046509, -1.2167118787765503, -1.884763479232788, 1.0944790840148926, 1.7142730951309204, 1.8920873403549194, 1.386167287826538, 0.15844112634658813, -1.5459941625595093, -0.9301481246948242, -0.0538637600839138, -0.833677351474762, -1.1472196578979492, -0.5956106185913086, -1.3884358406066895, 1.5047504901885986, -0.7407974004745483, -3.1609044075012207, -1.9678397178649902, -1.530045509338379, 0.3929499685764313, 1.6048074960708618, -0.0938672125339508, 0.014446491375565529, -1.288192629814148, -0.9931935667991638, 0.08309164643287659, 0.5911707878112793, -2.640700101852417, 1.348371148109436, -0.05540541186928749, -0.6300245523452759, -0.5897001028060913, -0.8095176219940186, 0.5634795427322388, -0.23818272352218628, -1.4308602809906006, -1.1426409482955933, 0.7048757076263428, -0.2618008255958557, 1.7248972654342651, -0.00566728413105011, -0.7385657429695129, 0.16934001445770264, -1.0479958057403564, 0.678706169128418, -0.5729792714118958, 1.0405242443084717, 0.127522274851799, 0.7178387641906738, -1.1736704111099243, -1.4704176187515259, 0.43914952874183655, -0.4794290065765381, 1.2575780153274536, -1.8450322151184082, -1.3823168277740479, -0.0025304313749074936, 1.1054096221923828, -0.2515498101711273, -2.33990478515625, 1.9135493040084839, -0.07369875907897949, -1.2662020921707153, -2.4571385383605957, 1.2121233940124512, -1.1168618202209473, 2.1422688961029053, 0.20469529926776886, 0.7019397020339966, -1.5162582397460938, -0.6286987662315369, -0.053046442568302155, 0.5970880389213562, -0.274273157119751, -0.45358169078826904, -1.6638449430465698, 0.7098968625068665, 0.28278517723083496, 0.5231764316558838, -0.3957032561302185, 1.2139911651611328, -2.0957183837890625, 0.17604003846645355, -0.8815881609916687, 0.1034555658698082, 0.6424606442451477, 0.8401890993118286, 1.5709071159362793, -0.6364938616752625, 2.6397929191589355, -0.7208391427993774, 1.0816856622695923, -1.4779410362243652, 2.277517795562744, 0.19235974550247192, 0.6462177038192749, -0.011391619220376015, -0.07730872184038162, -1.0100882053375244, -2.7020387649536133, 1.2263567447662354, -0.18621836602687836, 2.3048293590545654, -0.07306432723999023, 2.156001329421997, 0.40929532051086426, -0.7445467114448547, 0.9272005558013916, 0.9694026708602905, -1.2338542938232422, -0.5985312461853027, 0.4979028105735779, 0.41705945134162903, 0.4147370457649231, -2.1925594806671143, -1.1310235261917114, 0.8440234065055847, -1.6436741352081299, 0.6608390212059021, 0.7034006714820862, -0.6008576154708862, 0.05955575406551361, 0.30635353922843933, 0.259810209274292, 0.5620633363723755, -0.1445632129907608, 1.5006102323532104, 0.17657655477523804, -0.1838754415512085, 0.9759607911109924, -1.336050271987915, -1.3178670406341553, 0.3359467387199402, 0.29043519496917725, 1.826944351196289, -0.7200961709022522, -0.08379226177930832, 0.9899473786354065, -0.9944477081298828, 0.8776010870933533, -0.5931596159934998, 0.22415345907211304, 0.31520888209342957, -1.3767954111099243, -0.9343562126159668, -0.07928045839071274, 1.0100234746932983, -0.5218523740768433, -1.291630744934082, 1.352694034576416, -0.9403048753738403, -0.7047476768493652, 2.504195213317871, 0.6022015810012817, -1.616634488105774, -1.2718268632888794, 0.2762468457221985, 0.6731063723564148, -1.6260024309158325, 0.8422249555587769, 1.4556361436843872, 0.549264669418335, 0.4025838077068329, 0.4342503547668457, 1.076851725578308, 2.391422986984253, -0.6243330240249634, -1.2983641624450684, -1.7483470439910889, 0.6716263890266418, 0.8698210716247559, 0.7611477375030518, -1.5898511409759521, 1.529530644416809, -2.0494139194488525, -0.9545640349388123, 0.672527015209198, 0.8083449602127075, -0.5360766053199768, -0.28023895621299744, -0.060136377811431885, -0.1337953507900238, -0.2290695458650589, 1.1704295873641968, 0.05104539915919304, -1.6175795793533325, -0.25306186079978943, -1.3237359523773193, -1.4904534816741943, 0.2402241975069046, -1.2216962575912476, 0.2818860411643982, -0.3110548257827759, -1.3378783464431763, -0.4974493980407715, -0.3924957811832428, -0.9641960263252258, -0.27785009145736694, -1.7780267000198364, 0.43181151151657104, -0.5639820098876953, -1.5691121816635132, -0.5068035125732422, 1.1406227350234985, 0.1867091804742813, 0.6860585808753967, 1.7266530990600586, 1.3754472732543945, -0.34321320056915283, -1.1263118982315063, -0.336142897605896, -1.0765998363494873, 0.3590244948863983, -0.03256111964583397, 1.2443675994873047, 0.2664707601070404, 1.0979171991348267, 0.3836994767189026, 1.5945253372192383, -0.9787816405296326, 0.6233514547348022, 0.25684717297554016, -0.7422625422477722, 0.5898456573486328, -0.6937768459320068, 0.7158833742141724, 0.0941191017627716, -0.6962095499038696, 1.2891377210617065, 0.2647746205329895, -1.1761517524719238, 0.049233078956604004, -1.50534188747406, -0.5715383291244507, -1.6010926961898804, -0.6140256524085999, -0.30191582441329956, -1.2914106845855713, 0.2633931636810303, 1.5358966588974, -0.6395539045333862, -1.6704007387161255, -1.3335968255996704, 0.17715781927108765, 0.9665125608444214, 0.4892232418060303, -1.5845147371292114, 0.2665630280971527, 1.2599835395812988, -0.7439969182014465, 1.375579833984375, -0.23399674892425537, -0.04565019905567169, -0.8158296346664429, 0.5938637256622314, 0.04138951748609543, 0.6430358290672302, 1.083950400352478, -0.27834075689315796, 0.927085816860199, 0.10326866060495377, 0.4726864695549011, 0.1324739307165146, -1.182991862297058, 0.31088653206825256, 0.014408346265554428, 0.7980141043663025, 0.1154966726899147, 1.5684047937393188, 0.453401118516922, 2.2306602001190186, -0.27814924716949463, 0.2583429515361786, -0.18135035037994385, -0.33784735202789307, 0.1646009385585785, 0.0685671865940094, -2.0791399478912354, 0.42294424772262573, -0.902911901473999, 0.34969714283943176, 0.3860327899456024, -0.14100176095962524, 1.8890738487243652, -0.7225279808044434, 0.5272400379180908, -0.3568282127380371, 1.1871061325073242, 0.1431514173746109, -0.07413778454065323, -0.6981383562088013, -0.0037303026765584946, 1.8494497537612915, -0.7193478345870972, 2.1191952228546143, 0.392134428024292, 0.10731696337461472, -0.3707856833934784, 1.422970175743103, -0.5189794898033142, 0.5043716430664062, 1.24215829372406, 0.9503442645072937, -0.6369106769561768, -0.5478856563568115, -0.22564241290092468, 0.15660256147384644, 1.4896762371063232, 0.9423323273658752, -1.1791608333587646, -1.0128179788589478, 1.1221661567687988, -0.25093957781791687, -0.9290352463722229, -0.38120949268341064, 0.9651955366134644, 0.6338001489639282, -1.196611762046814, -1.7573168277740479, 1.8010683059692383, -1.9172394275665283, 0.6358168125152588, -1.8375028371810913, -0.3216865062713623, -1.3653329610824585, -1.735976219177246, 0.5160931944847107, 1.1848491430282593, 0.6448425054550171, 2.2446701526641846, 1.1365478038787842, -1.8493680953979492, 0.4994947612285614, 0.40352335572242737, 0.6215800046920776, -2.1089539527893066, -1.265620470046997, 2.0043368339538574, -0.07650401443243027, -0.07330071926116943, -0.6699921488761902, 0.3808633089065552, -3.1654622554779053, -1.4893062114715576, -2.086634874343872, -1.3015868663787842, 0.4829140901565552, 0.20592011511325836, -0.1117359846830368, -0.9208534359931946, 2.358025312423706, -1.3179123401641846, -0.2816240191459656, 2.0315911769866943, 1.1762288808822632, -0.16646647453308105, -1.1506353616714478, 0.2696559429168701, -0.5964003801345825, -1.5601403713226318, 1.5986411571502686, 1.7165294885635376, 1.5330419540405273, -0.7704847455024719, 3.8874664306640625, -0.4696517884731293, 0.5057021379470825, 0.6648915410041809, 1.7003742456436157, -0.18458665907382965, -0.6868480443954468, 0.6927555799484253, -0.048778779804706573, -0.8755130171775818, -0.3304232656955719, -0.6422710418701172, 0.04335760325193405, 0.180059015750885, -0.468524307012558, 0.024891257286071777, 0.5402524471282959, -0.4616308808326721, -0.5706627368927002, 1.6899409294128418, -0.39132118225097656, -0.060191504657268524, -0.6066865921020508, 0.14159570634365082, 0.4438058137893677, -0.7319074273109436, -1.1364476680755615, 0.19102080166339874, 0.026246868073940277, -0.23193910717964172, -1.9769115447998047, 0.4983759820461273, 0.5279264450073242, 0.5689533352851868, -2.1206979751586914, 0.34669628739356995, 0.7002028822898865, -0.4836770296096802, 0.7598353624343872, -0.49306127429008484, -0.9902405738830566, 2.585679531097412, -0.16504405438899994, -0.11126528680324554, 0.20492668449878693, 0.731106698513031, 2.073225259780884, 0.04192519187927246, -0.2610241174697876, -1.3524868488311768, -0.027337510138750076]</t>
+  </si>
+  <si>
     <t>Трамп Дональдович</t>
   </si>
   <si>
@@ -279,6 +291,9 @@
     <t>S23007815</t>
   </si>
   <si>
+    <t>[0.9936350584030151, -0.49836409091949463, -0.3832937777042389, 0.17103466391563416, 0.6883322596549988, -1.0855408906936646, -0.1830907016992569, 0.04269116371870041, 0.27693918347358704, -0.1264360398054123, 2.7856085300445557, 0.47162121534347534, 1.1398327350616455, 0.1540234386920929, -0.06751683354377747, 0.11085126549005508, -0.9979975819587708, 0.17097653448581696, -1.5904120206832886, 1.5914478302001953, -0.3683832585811615, -1.4243249893188477, 0.783075749874115, -2.471554756164551, -2.094402313232422, -0.12905137240886688, 0.13049396872520447, -1.0098350048065186, -0.5649203062057495, -0.8974714279174805, 0.9623892903327942, 0.7350187301635742, -0.390837162733078, 1.344311237335205, -1.036614179611206, -1.2161370515823364, 1.4863462448120117, -0.7114652395248413, -1.3641936779022217, 0.515215277671814, -1.2477397918701172, 0.0819973573088646, 0.9835690855979919, 0.9981339573860168, 0.6171723008155823, 0.2904999852180481, 1.3823107481002808, 1.7783254384994507, -1.7572399377822876, -0.9370962977409363, -0.9040223956108093, -0.6773573756217957, 0.3773689866065979, 0.43526363372802734, 0.24186009168624878, -0.15469202399253845, -1.3182882070541382, 0.53622967004776, -0.829555094242096, 0.25894567370414734, -0.9875105619430542, 1.2833740711212158, -2.0549981594085693, 0.44560280442237854, 0.21745231747627258, -0.12461700290441513, -0.4949389398097992, -1.2103174924850464, 0.5784095525741577, -1.1070119142532349, 0.21292945742607117, -0.3282325863838196, -0.07153458893299103, 0.18791654706001282, -0.7991927266120911, -1.4842551946640015, 0.6643844842910767, -1.6790350675582886, -0.9451213479042053, -0.4816417694091797, -0.062471888959407806, 2.2052886486053467, 0.568630039691925, -0.18638944625854492, -0.24057844281196594, 1.2073408365249634, -0.21502676606178284, 0.1597123146057129, -0.6503413319587708, -0.2375689595937729, 0.15073132514953613, 0.14025530219078064, 0.5130614638328552, -2.0596728324890137, -0.011962857097387314, 2.0778822898864746, 0.4539566934108734, 1.873361349105835, 0.6233695149421692, -0.5574933290481567, -1.1280269622802734, 1.4009449481964111, -0.10276566445827484, 1.3074113130569458, -0.5246127247810364, -0.63988196849823, 0.20368517935276031, -0.9615427255630493, -1.6316521167755127, -0.7560130953788757, 1.5761795043945312, 0.730050802230835, -0.8002814650535583, -0.14618149399757385, 0.5168378949165344, 1.5776981115341187, 1.6346131563186646, 0.2012280523777008, 0.5456932187080383, 0.7118035554885864, -0.29477864503860474, 0.9284364581108093, 1.094416618347168, -0.5156838297843933, -0.39353764057159424, -1.1985071897506714, -0.08513621985912323, -1.7279057502746582, 0.09611838310956955, -1.9855544567108154, -0.09676310420036316, 0.8988884687423706, 0.705001711845398, 0.9059971570968628, -0.4555530250072479, -0.7898144125938416, -1.6761668920516968, -2.0470004081726074, 0.805689811706543, 0.4242781698703766, 0.2748169004917145, 0.5248039364814758, -2.2368569374084473, 1.0620629787445068, 0.6161758899688721, 0.1466694474220276, -0.797181248664856, 1.072383999824524, 0.6504020094871521, 1.221618413925171, 1.4279340505599976, 0.5522960424423218, -1.4334989786148071, 1.7146477699279785, 0.03449957072734833, -0.10987581312656403, -1.3968580961227417, -0.7242648005485535, -0.5113358497619629, -1.6526951789855957, 1.4554359912872314, 0.8759623765945435, 0.3240269124507904, -0.15875700116157532, 0.5178413391113281, 0.8232685923576355, -1.3906538486480713, 0.2498292773962021, -0.8654167056083679, 0.4731561839580536, -0.5002102255821228, 0.739287793636322, -0.9725330471992493, -0.47086185216903687, 0.6804958581924438, 0.1601303219795227, -0.7378705143928528, 0.6466742753982544, 0.10937050729990005, 0.6105529069900513, 0.8422613739967346, 0.4801173508167267, -0.31587308645248413, -0.47514989972114563, 0.8526877760887146, 0.6745021939277649, -0.36103200912475586, 0.8499017953872681, 2.1372478008270264, 0.8175026178359985, 0.19939468801021576, 0.25520631670951843, 0.2287825345993042, -0.6035057306289673, 0.26704198122024536, 1.2047250270843506, 0.7263349890708923, 0.7328020930290222, -0.420368492603302, -0.5669986009597778, 1.5541255474090576, -2.1589643955230713, 0.5575435757637024, -0.4695034623146057, 1.0353177785873413, 2.0747756958007812, 0.03053765371441841, 0.6421033143997192, -0.01033291406929493, 1.1155439615249634, 0.06840583682060242, 0.24666349589824677, 1.1194173097610474, -0.447703093290329, -0.2545534670352936, 0.07482913136482239, 0.01585432142019272, 0.2409777194261551, -0.5205453038215637, -0.15232275426387787, -1.3461759090423584, -1.3731344938278198, 1.016880750656128, -0.9467265009880066, 0.3274241089820862, 1.6224838495254517, 1.2517396211624146, 1.443434715270996, -0.9561821222305298, -0.15324926376342773, 0.3524359464645386, 0.6700736880302429, -0.386586993932724, -0.3140881359577179, -0.5093973875045776, 0.02451595477759838, -0.9979932904243469, 0.3713429272174835, 1.9194945096969604, -0.2508615255355835, 1.0629221200942993, 1.526644229888916, 0.5855132341384888, -0.2076079100370407, -1.041550636291504, -0.2650531232357025, -0.47260481119155884, 0.7546268105506897, -1.2706959247589111, 1.8217278718948364, -1.1626427173614502, 0.2751937508583069, 1.7697890996932983, -0.7505213618278503, 0.5191516280174255, 0.21674644947052002, -0.7752541899681091, 0.2661813497543335, 0.9583603739738464, -0.34348538517951965, -0.3924080431461334, -1.1546976566314697, 0.49036064743995667, -0.4201754629611969, -0.7731917500495911, -0.19806146621704102, 0.13794556260108948, 0.2926580011844635, 0.7508496046066284, -2.5513079166412354, 0.016213860362768173, 1.4575538635253906, 1.3672459125518799, -0.08134125173091888, 0.05252744257450104, 0.016624022275209427, 1.0081297159194946, 1.1599427461624146, 1.3149229288101196, 1.0753389596939087, -1.502092957496643, 1.2275583744049072, -0.013742152601480484, -0.6575844287872314, 0.37435081601142883, -1.154712200164795, 1.806171178817749, 0.5687049627304077, -0.26475685834884644, 0.22201712429523468, 0.4638538062572479, 0.5275869965553284, -0.5735592842102051, 2.5931777954101562, 0.732746422290802, 0.227286696434021, -1.0126591920852661, -0.6705788373947144, 0.7341222763061523, -0.8345006108283997, -0.6619595289230347, 0.8418402075767517, -0.8002698421478271, -0.29827848076820374, 1.7640464305877686, 0.8197200894355774, -0.6447325348854065, 0.0889197587966919, -0.7744061350822449, 1.6745706796646118, -0.6326844096183777, 1.346731185913086, 0.7194600701332092, -0.08972882479429245, 0.6488691568374634, 1.6335242986679077, -0.5384290218353271, 0.6856478452682495, 1.5782688856124878, 1.1641051769256592, 0.03268665447831154, -0.1931055784225464, -0.0018484601750969887, 1.345263123512268, -0.014760889112949371, -0.5870139002799988, -0.18918511271476746, 2.1478652954101562, -0.537085235118866, -0.04748228192329407, 0.8437657356262207, 0.9568455815315247, -0.30056875944137573, 0.6637187600135803, 0.10670047998428345, 0.15204918384552002, 0.5195221900939941, -0.405426561832428, 0.2095373570919037, -0.3071006238460541, 1.3344634771347046, -0.6841026544570923, -0.6230317950248718, -0.08173537254333496, 0.2933511435985565, 0.21024435758590698, -0.19516736268997192, 0.2391640543937683, 1.3882683515548706, 0.1669917106628418, 0.1460736244916916, -0.856643557548523, 2.226285457611084, 0.14359349012374878, 1.2974202632904053, 0.03131191432476044, 0.016314689069986343, -0.42849376797676086, 0.08020896464586258, 1.209298849105835, -0.1252380758523941, -1.20543372631073, -0.4899721145629883, -1.614547848701477, -0.10891426354646683, -0.7119759917259216, -1.670694351196289, -0.7890399694442749, 0.83409583568573, -0.7471232414245605, 0.45454907417297363, -0.7118582725524902, -1.492038369178772, -0.15036779642105103, -0.907913863658905, 2.7495129108428955, 1.1761047840118408, 0.8331257104873657, 0.7405511140823364, 0.3261725604534149, -1.6557421684265137, -1.9474610090255737, 0.0628441870212555, -0.9032959342002869, -0.1486988365650177, -0.8388379812240601, 0.8753883838653564, -0.25417283177375793, -0.07257124036550522, -1.1330498456954956, -0.6034825444221497, 1.2361100912094116, 0.9183297753334045, 1.2077250480651855, 1.5164902210235596, 1.128494381904602, 0.9492988586425781, 2.4692580699920654, 0.9474177360534668, -1.948033094406128, 0.8806105852127075, -0.09798477590084076, 1.4182113409042358, 0.09861597418785095, 0.33477693796157837, 0.1734132170677185, -1.634252667427063, -1.1956944465637207, -0.5944390892982483, 0.1281071901321411, 1.3718888759613037, -0.7234360575675964, 0.18631893396377563, -1.0648205280303955, -0.1914767324924469, 1.1942927837371826, 1.4322364330291748, 1.1350654363632202, -0.3508128821849823, -0.09881280362606049, 0.9464432597160339, 0.6805686354637146, -0.6464476585388184, 0.9687580466270447, -1.2249906063079834, 1.3910002708435059, -0.3130297362804413, 0.49774879217147827, 0.9183410406112671, -0.44510364532470703, -0.8170068860054016, 1.2982851266860962, -0.2125578075647354, -0.03883502632379532, 0.47351861000061035, 1.1160563230514526, -0.9558190107345581, -0.6307080984115601, -0.9974913597106934, 0.5205649733543396, -0.6401940584182739, 0.2543989419937134, 0.10282120108604431, 2.226414442062378, 0.6897554397583008, 0.7601025700569153, 0.9496942162513733, -1.4431164264678955, 0.7645776271820068, -0.04071585088968277, -0.7835664749145508, 0.7475156188011169, 0.11069242656230927, -0.5443031787872314, 0.5243321657180786, 1.364188313484192, -0.4964122474193573, -0.8103589415550232, 0.9673190712928772, -1.2181224822998047, 1.5501505136489868, 0.4522012174129486, 0.3499658405780792, -1.2561776638031006, -1.5509603023529053, -1.4645450115203857, 0.3483273684978485, 1.076517939567566, 0.05297176539897919, 2.5751285552978516, 1.622496247291565, 1.5372637510299683, -0.018714791163802147, -0.4766213297843933, -0.34737834334373474, 0.23909029364585876, -0.17202547192573547, 0.09490732103586197, 0.7388318181037903, 0.5645279288291931, -1.3329508304595947, 0.33704978227615356, -0.20448048412799835, 1.0787222385406494, -1.10955011844635, -0.40845027565956116, -0.5657618641853333, 1.7420217990875244, 0.878247857093811, -1.6031572818756104, -0.5812610983848572, 0.020081592723727226, -1.0526683330535889, 0.4183802902698517, 1.682739019393921, -1.1578261852264404, 0.41216450929641724, -0.32232969999313354, 1.5552233457565308, -0.4671477675437927, -1.2206671237945557, -0.6870539784431458, -2.9131734371185303, -1.329901933670044, -1.3265682458877563, 1.33900785446167, -0.6902883648872375, -0.506458044052124, 0.10976570844650269, 0.24872705340385437, 1.5188872814178467, 0.6447558999061584]</t>
+  </si>
+  <si>
     <t>Твенти Уан Пилотсович</t>
   </si>
   <si>
@@ -334,12 +349,15 @@
   <si>
     <t>Best Group</t>
   </si>
+  <si>
+    <t>[0.8925038576126099, -0.7687393426895142, 0.5704202055931091, 0.2120499461889267, 0.4517909586429596, -0.43394148349761963, 0.5699537992477417, -0.9256817102432251, -0.19992387294769287, 0.7018370628356934, 1.9448240995407104, 0.3643888235092163, -0.4833279252052307, 0.5212052464485168, 1.3080328702926636, -0.8697160482406616, -0.11798633635044098, 0.7520568370819092, -0.8283511400222778, -0.004868552088737488, -0.88823002576828, -2.043701171875, 1.6123225688934326, -1.9304556846618652, -1.5517690181732178, -0.9306477904319763, -0.9343650341033936, -1.1890738010406494, 0.0020105764269828796, -1.5872581005096436, 0.0037171095609664917, 0.9382524490356445, -0.5045737028121948, 0.5758123397827148, -0.961195707321167, -0.7616714239120483, 0.9032834768295288, -0.14143502712249756, -1.8686074018478394, 0.9137747287750244, -0.6230596303939819, -0.38203129172325134, -1.6632232666015625, 0.9822949767112732, 1.398577094078064, 0.15052065253257751, 2.2371714115142822, 0.14408570528030396, 0.24896828830242157, -0.8495228290557861, -0.1147524043917656, -0.9461892247200012, -0.6788454055786133, 0.39755678176879883, -0.26662325859069824, -0.17008766531944275, -0.8348166942596436, 0.5204288363456726, -0.9329736232757568, 0.0444362536072731, -2.78674578666687, 0.010139035061001778, -2.103881359100342, 0.5489279627799988, 1.198458194732666, -0.4985952377319336, -0.8444714546203613, -0.8529084920883179, -0.993062436580658, -1.5858088731765747, 0.39519307017326355, 1.7204021215438843, -0.4348970651626587, -0.8912901878356934, 0.24201634526252747, -1.5610848665237427, 1.1085731983184814, -0.6938727498054504, -0.45480984449386597, 0.569223165512085, -0.24911926686763763, 0.8630439639091492, 0.36535724997520447, -0.10201496630907059, 0.6916993260383606, 2.301790475845337, -0.7039280533790588, 1.0798227787017822, 0.35909903049468994, 1.3482424020767212, 0.39855286478996277, 0.04273858666419983, -0.25485050678253174, -1.509373426437378, -0.006783135235309601, 0.48025524616241455, -0.2323625683784485, 2.794102191925049, 0.3277195394039154, -0.2669591009616852, 0.5605296492576599, 0.31190207600593567, 0.14938139915466309, 0.43172258138656616, 0.6449044942855835, -0.0790974423289299, -0.008939094841480255, -1.1662424802780151, -1.6776854991912842, -0.7890796065330505, 0.7182208895683289, 0.48131224513053894, -0.39370810985565186, 0.08098574727773666, -1.2673863172531128, 1.3012564182281494, 1.3829833269119263, -1.1764285564422607, 0.5161668062210083, 1.9677106142044067, 0.10109294950962067, -0.13799969851970673, 0.25285062193870544, 0.32308530807495117, 0.11795015633106232, -1.6076138019561768, 1.01767897605896, -1.5230110883712769, 0.7166168689727783, -2.2976911067962646, 0.726485013961792, 0.06071298196911812, 0.9313749670982361, 1.7455906867980957, 0.7263433933258057, -0.1630568653345108, -1.1964038610458374, -1.458483338356018, -0.04180114343762398, -0.10188473761081696, -0.24761919677257538, 2.3892204761505127, -1.3699043989181519, 1.5926084518432617, 0.46848297119140625, 0.8217263221740723, -0.7574796080589294, 1.1409927606582642, 1.0136792659759521, 1.407813549041748, 0.6471772789955139, 1.0972768068313599, -0.9406450986862183, 0.5639133453369141, 0.17546503245830536, 0.5964224338531494, -1.2780967950820923, -0.10582923144102097, 0.15076681971549988, -1.6010923385620117, 0.5991489887237549, -0.18841896951198578, -0.9963156580924988, 0.6093962788581848, -1.0954784154891968, 0.33683115243911743, -0.7235226631164551, 0.06647667288780212, -0.46523991227149963, 0.23479443788528442, -1.094365119934082, -0.8019445538520813, -1.0148557424545288, -0.840924859046936, -0.8986725211143494, 1.0261213779449463, -0.9594253897666931, 0.3342779278755188, -0.10092899203300476, -0.19586676359176636, 2.0642330646514893, -0.5069578886032104, 0.3379647731781006, 1.6850268840789795, 1.1333508491516113, -0.5771239995956421, 0.43871721625328064, 0.42908912897109985, 1.2235732078552246, 0.9791344404220581, -0.24024741351604462, 1.0255768299102783, 0.18764372169971466, 0.4673757553100586, 0.16875620186328888, 0.9102680683135986, -0.7696326375007629, -0.25956255197525024, 0.1525699347257614, -0.6791226267814636, 0.9374894499778748, -1.6542118787765503, 0.7678937315940857, -0.23402483761310577, 0.21714890003204346, 0.5353483557701111, 0.5613757967948914, 1.2906122207641602, 2.0633580684661865, 0.7028692960739136, -1.524924635887146, -0.5108891725540161, 0.15262176096439362, -1.1338979005813599, -1.2530986070632935, -0.8721039891242981, -0.028985872864723206, 0.2824459969997406, -0.2691699266433716, 2.6711885929107666, -0.012798704206943512, 0.7346149682998657, 0.9902796149253845, -0.7398685812950134, -0.6962575912475586, 0.9760335087776184, -0.3052171468734741, 1.1937391757965088, -1.666569471359253, 0.6568727493286133, -1.1407662630081177, 0.4595094323158264, -1.303999900817871, -0.08017188310623169, -0.24171322584152222, -0.48391661047935486, 0.661810040473938, 0.755149781703949, 1.2883151769638062, 0.4406023919582367, -0.25082921981811523, 0.7227957248687744, 0.04138163477182388, 0.8618679046630859, -1.3857969045639038, -1.3650178909301758, -1.2945187091827393, -0.5757430791854858, -0.10993734002113342, 1.580013632774353, 1.5212088823318481, 0.7436646819114685, 1.5431795120239258, -0.8510051369667053, -1.9265474081039429, 0.8440430164337158, -0.9154101014137268, 0.9126276969909668, 0.8661890625953674, -0.2888386845588684, 0.1050441786646843, 0.8028907775878906, 0.5255529880523682, 1.4725922346115112, 0.4896540641784668, 0.29296445846557617, 0.47436797618865967, -0.6322063207626343, 0.40438538789749146, -2.0847015380859375, -0.6984430551528931, 0.8353896737098694, 0.4265541434288025, -0.5719545483589172, -1.138786792755127, -1.5384492874145508, -1.3353791236877441, -0.1944153755903244, 0.9656756520271301, 1.3902430534362793, -1.3114168643951416, 1.663756012916565, -1.1658929586410522, 0.0658213421702385, 0.9376325607299805, 0.2071092426776886, 0.8905631303787231, 0.9004421234130859, 1.1638017892837524, -1.4565598964691162, 0.4824386239051819, 0.2821733355522156, 1.192659616470337, 1.419891357421875, 0.3394103944301605, -0.14162522554397583, 0.11027580499649048, -0.04056370258331299, 0.9610684514045715, -1.2667603492736816, -1.2417765855789185, 1.2728570699691772, -1.0625207424163818, 0.06724464148283005, 1.6721537113189697, -0.7834770679473877, 0.2583325505256653, 0.657871425151825, -0.10212111473083496, 1.3515428304672241, -0.6362581253051758, 1.592186689376831, 0.2900881767272949, -0.12942759692668915, 1.797249674797058, 0.531444251537323, 0.48338979482650757, 0.6307298541069031, 0.3024630844593048, 0.32345345616340637, 0.6843798160552979, 0.10834702849388123, 0.7717282176017761, 0.8089597225189209, 1.04501211643219, -2.1665728092193604, -0.12991496920585632, 1.693666696548462, 0.3028571605682373, 0.28399857878685, -0.8869582414627075, 2.1105918884277344, 0.3057849407196045, 0.08342228084802628, -0.89913010597229, 0.8596949577331543, -0.2675636112689972, 0.6098544597625732, -0.6250513195991516, -0.16463376581668854, -0.11989564448595047, 0.0961439311504364, -1.483622431755066, 0.9364970922470093, 0.6119147539138794, 1.4370800256729126, -0.08835496753454208, 0.43712955713272095, 1.433220624923706, 0.037163227796554565, 1.83164644241333, -0.883986234664917, 0.512432336807251, -0.060364555567502975, 1.1337127685546875, 0.562580406665802, -0.33308833837509155, 0.7156866192817688, 0.06014586612582207, 0.19337555766105652, -1.0627148151397705, -1.3060498237609863, -0.5539803504943848, 0.17691996693611145, 0.2509324252605438, -1.0419032573699951, 0.22000011801719666, -0.6652830243110657, 0.6546972990036011, 0.3881102502346039, -0.4054393768310547, -1.5788904428482056, -0.6545238494873047, 0.449440062046051, -0.4699351489543915, 1.0958541631698608, 1.4263339042663574, 0.6091220378875732, -0.7970655560493469, -0.07528501749038696, -1.5297795534133911, -1.9564640522003174, -1.3104482889175415, 0.8240982294082642, -0.27772843837738037, 0.008506907150149345, -0.7627095580101013, 0.6727111339569092, -0.24707764387130737, -1.0084489583969116, -1.5023493766784668, 0.5632971525192261, 0.9922354817390442, 0.8179942965507507, 1.4550726413726807, -0.14527089893817902, 0.06150529533624649, 0.04987283796072006, -0.013830485753715038, -1.3193484544754028, -0.4272303283214569, 0.10377627611160278, 1.0045608282089233, 0.37107303738594055, 0.9060239791870117, -0.32099810242652893, -0.654277503490448, -1.2220791578292847, -0.3864199221134186, 0.1947256177663803, 0.6942713856697083, -0.853001594543457, -1.2425018548965454, -0.34424662590026855, 0.6893113851547241, 1.577171802520752, 0.933385968208313, 0.9301478862762451, -1.2039673328399658, -0.40161773562431335, 0.3265014886856079, 0.9803699254989624, -0.08417840301990509, 1.601674199104309, -1.189946174621582, 1.2445282936096191, -0.35173481702804565, -0.12006553262472153, -0.18874527513980865, -1.1838573217391968, -0.7502593994140625, 1.8099298477172852, 0.7894874215126038, -0.28211718797683716, -0.9719375371932983, 0.7064939737319946, -1.3071844577789307, -0.4977387487888336, -1.4372485876083374, -0.4240274429321289, -0.14294052124023438, 0.2801375389099121, 1.146712303161621, 0.5404306650161743, 0.7215015292167664, -0.7601815462112427, 2.276383638381958, -0.9901136755943298, -1.287948489189148, 0.16470521688461304, -0.4047406315803528, 1.373852014541626, 0.9240980744361877, 0.26579970121383667, 0.7914238572120667, 1.388283371925354, 0.10207673907279968, 1.259653091430664, 1.7182501554489136, -1.5374352931976318, 1.0048680305480957, 1.4090673923492432, 0.8095342516899109, -1.4435511827468872, -1.3171554803848267, -1.3423259258270264, -0.3911365568637848, 1.7124437093734741, 1.3781013488769531, 1.1859097480773926, 0.8722618222236633, -0.38299235701560974, 0.422318696975708, -0.011516386643052101, 0.7588923573493958, -1.082742691040039, 0.716332197189331, -0.35287946462631226, 1.3140641450881958, 1.4542208909988403, -0.04166918992996216, 1.0153582096099854, -0.7885770201683044, 0.3473524749279022, 0.4926931858062744, 0.00919070839881897, 0.15779449045658112, 0.18374985456466675, 2.1476097106933594, -1.0244166851043701, -1.2089241743087769, -0.7881772518157959, -1.1072643995285034, -0.312153697013855, 0.39828070998191833, -1.6747769117355347, -0.09921771287918091, 0.4792262613773346, 0.9906851649284363, 0.26798883080482483, -1.327502727508545, -1.3028984069824219, -1.0162062644958496, -0.4061952531337738, -1.5005353689193726, 1.3108587265014648, -1.4591939449310303, 0.7984908819198608, 0.5982048511505127, -2.146425724029541, -0.36861371994018555, 0.9594817757606506]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -355,7 +373,11 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -386,18 +408,21 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,6 +646,7 @@
     <col customWidth="1" min="4" max="4" width="33.71"/>
     <col customWidth="1" min="5" max="5" width="15.86"/>
     <col customWidth="1" min="6" max="6" width="9.57"/>
+    <col customWidth="1" min="7" max="7" width="10270.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -642,105 +668,123 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" ht="30.75" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
+      <c r="A2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="D2" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3">
         <v>8348.0</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" ht="21.0" customHeight="1">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
+      <c r="A3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3">
         <v>8349.0</v>
       </c>
+      <c r="G3" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>16</v>
+      <c r="A4" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3">
         <v>8350.0</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" ht="17.25" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
+      <c r="A5" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3">
         <v>8352.0</v>
       </c>
+      <c r="G5" s="4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" ht="17.25" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>28</v>
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F6" s="3">
         <v>8352.0</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" ht="17.25" customHeight="1">
@@ -767,6 +811,986 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
     </row>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="34" ht="15.75" customHeight="1"/>
+    <row r="35" ht="15.75" customHeight="1"/>
+    <row r="36" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
+    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="39" ht="15.75" customHeight="1"/>
+    <row r="40" ht="15.75" customHeight="1"/>
+    <row r="41" ht="15.75" customHeight="1"/>
+    <row r="42" ht="15.75" customHeight="1"/>
+    <row r="43" ht="15.75" customHeight="1"/>
+    <row r="44" ht="15.75" customHeight="1"/>
+    <row r="45" ht="15.75" customHeight="1"/>
+    <row r="46" ht="15.75" customHeight="1"/>
+    <row r="47" ht="15.75" customHeight="1"/>
+    <row r="48" ht="15.75" customHeight="1"/>
+    <row r="49" ht="15.75" customHeight="1"/>
+    <row r="50" ht="15.75" customHeight="1"/>
+    <row r="51" ht="15.75" customHeight="1"/>
+    <row r="52" ht="15.75" customHeight="1"/>
+    <row r="53" ht="15.75" customHeight="1"/>
+    <row r="54" ht="15.75" customHeight="1"/>
+    <row r="55" ht="15.75" customHeight="1"/>
+    <row r="56" ht="15.75" customHeight="1"/>
+    <row r="57" ht="15.75" customHeight="1"/>
+    <row r="58" ht="15.75" customHeight="1"/>
+    <row r="59" ht="15.75" customHeight="1"/>
+    <row r="60" ht="15.75" customHeight="1"/>
+    <row r="61" ht="15.75" customHeight="1"/>
+    <row r="62" ht="15.75" customHeight="1"/>
+    <row r="63" ht="15.75" customHeight="1"/>
+    <row r="64" ht="15.75" customHeight="1"/>
+    <row r="65" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
+    <row r="81" ht="15.75" customHeight="1"/>
+    <row r="82" ht="15.75" customHeight="1"/>
+    <row r="83" ht="15.75" customHeight="1"/>
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1"/>
+    <row r="86" ht="15.75" customHeight="1"/>
+    <row r="87" ht="15.75" customHeight="1"/>
+    <row r="88" ht="15.75" customHeight="1"/>
+    <row r="89" ht="15.75" customHeight="1"/>
+    <row r="90" ht="15.75" customHeight="1"/>
+    <row r="91" ht="15.75" customHeight="1"/>
+    <row r="92" ht="15.75" customHeight="1"/>
+    <row r="93" ht="15.75" customHeight="1"/>
+    <row r="94" ht="15.75" customHeight="1"/>
+    <row r="95" ht="15.75" customHeight="1"/>
+    <row r="96" ht="15.75" customHeight="1"/>
+    <row r="97" ht="15.75" customHeight="1"/>
+    <row r="98" ht="15.75" customHeight="1"/>
+    <row r="99" ht="15.75" customHeight="1"/>
+    <row r="100" ht="15.75" customHeight="1"/>
+    <row r="101" ht="15.75" customHeight="1"/>
+    <row r="102" ht="15.75" customHeight="1"/>
+    <row r="103" ht="15.75" customHeight="1"/>
+    <row r="104" ht="15.75" customHeight="1"/>
+    <row r="105" ht="15.75" customHeight="1"/>
+    <row r="106" ht="15.75" customHeight="1"/>
+    <row r="107" ht="15.75" customHeight="1"/>
+    <row r="108" ht="15.75" customHeight="1"/>
+    <row r="109" ht="15.75" customHeight="1"/>
+    <row r="110" ht="15.75" customHeight="1"/>
+    <row r="111" ht="15.75" customHeight="1"/>
+    <row r="112" ht="15.75" customHeight="1"/>
+    <row r="113" ht="15.75" customHeight="1"/>
+    <row r="114" ht="15.75" customHeight="1"/>
+    <row r="115" ht="15.75" customHeight="1"/>
+    <row r="116" ht="15.75" customHeight="1"/>
+    <row r="117" ht="15.75" customHeight="1"/>
+    <row r="118" ht="15.75" customHeight="1"/>
+    <row r="119" ht="15.75" customHeight="1"/>
+    <row r="120" ht="15.75" customHeight="1"/>
+    <row r="121" ht="15.75" customHeight="1"/>
+    <row r="122" ht="15.75" customHeight="1"/>
+    <row r="123" ht="15.75" customHeight="1"/>
+    <row r="124" ht="15.75" customHeight="1"/>
+    <row r="125" ht="15.75" customHeight="1"/>
+    <row r="126" ht="15.75" customHeight="1"/>
+    <row r="127" ht="15.75" customHeight="1"/>
+    <row r="128" ht="15.75" customHeight="1"/>
+    <row r="129" ht="15.75" customHeight="1"/>
+    <row r="130" ht="15.75" customHeight="1"/>
+    <row r="131" ht="15.75" customHeight="1"/>
+    <row r="132" ht="15.75" customHeight="1"/>
+    <row r="133" ht="15.75" customHeight="1"/>
+    <row r="134" ht="15.75" customHeight="1"/>
+    <row r="135" ht="15.75" customHeight="1"/>
+    <row r="136" ht="15.75" customHeight="1"/>
+    <row r="137" ht="15.75" customHeight="1"/>
+    <row r="138" ht="15.75" customHeight="1"/>
+    <row r="139" ht="15.75" customHeight="1"/>
+    <row r="140" ht="15.75" customHeight="1"/>
+    <row r="141" ht="15.75" customHeight="1"/>
+    <row r="142" ht="15.75" customHeight="1"/>
+    <row r="143" ht="15.75" customHeight="1"/>
+    <row r="144" ht="15.75" customHeight="1"/>
+    <row r="145" ht="15.75" customHeight="1"/>
+    <row r="146" ht="15.75" customHeight="1"/>
+    <row r="147" ht="15.75" customHeight="1"/>
+    <row r="148" ht="15.75" customHeight="1"/>
+    <row r="149" ht="15.75" customHeight="1"/>
+    <row r="150" ht="15.75" customHeight="1"/>
+    <row r="151" ht="15.75" customHeight="1"/>
+    <row r="152" ht="15.75" customHeight="1"/>
+    <row r="153" ht="15.75" customHeight="1"/>
+    <row r="154" ht="15.75" customHeight="1"/>
+    <row r="155" ht="15.75" customHeight="1"/>
+    <row r="156" ht="15.75" customHeight="1"/>
+    <row r="157" ht="15.75" customHeight="1"/>
+    <row r="158" ht="15.75" customHeight="1"/>
+    <row r="159" ht="15.75" customHeight="1"/>
+    <row r="160" ht="15.75" customHeight="1"/>
+    <row r="161" ht="15.75" customHeight="1"/>
+    <row r="162" ht="15.75" customHeight="1"/>
+    <row r="163" ht="15.75" customHeight="1"/>
+    <row r="164" ht="15.75" customHeight="1"/>
+    <row r="165" ht="15.75" customHeight="1"/>
+    <row r="166" ht="15.75" customHeight="1"/>
+    <row r="167" ht="15.75" customHeight="1"/>
+    <row r="168" ht="15.75" customHeight="1"/>
+    <row r="169" ht="15.75" customHeight="1"/>
+    <row r="170" ht="15.75" customHeight="1"/>
+    <row r="171" ht="15.75" customHeight="1"/>
+    <row r="172" ht="15.75" customHeight="1"/>
+    <row r="173" ht="15.75" customHeight="1"/>
+    <row r="174" ht="15.75" customHeight="1"/>
+    <row r="175" ht="15.75" customHeight="1"/>
+    <row r="176" ht="15.75" customHeight="1"/>
+    <row r="177" ht="15.75" customHeight="1"/>
+    <row r="178" ht="15.75" customHeight="1"/>
+    <row r="179" ht="15.75" customHeight="1"/>
+    <row r="180" ht="15.75" customHeight="1"/>
+    <row r="181" ht="15.75" customHeight="1"/>
+    <row r="182" ht="15.75" customHeight="1"/>
+    <row r="183" ht="15.75" customHeight="1"/>
+    <row r="184" ht="15.75" customHeight="1"/>
+    <row r="185" ht="15.75" customHeight="1"/>
+    <row r="186" ht="15.75" customHeight="1"/>
+    <row r="187" ht="15.75" customHeight="1"/>
+    <row r="188" ht="15.75" customHeight="1"/>
+    <row r="189" ht="15.75" customHeight="1"/>
+    <row r="190" ht="15.75" customHeight="1"/>
+    <row r="191" ht="15.75" customHeight="1"/>
+    <row r="192" ht="15.75" customHeight="1"/>
+    <row r="193" ht="15.75" customHeight="1"/>
+    <row r="194" ht="15.75" customHeight="1"/>
+    <row r="195" ht="15.75" customHeight="1"/>
+    <row r="196" ht="15.75" customHeight="1"/>
+    <row r="197" ht="15.75" customHeight="1"/>
+    <row r="198" ht="15.75" customHeight="1"/>
+    <row r="199" ht="15.75" customHeight="1"/>
+    <row r="200" ht="15.75" customHeight="1"/>
+    <row r="201" ht="15.75" customHeight="1"/>
+    <row r="202" ht="15.75" customHeight="1"/>
+    <row r="203" ht="15.75" customHeight="1"/>
+    <row r="204" ht="15.75" customHeight="1"/>
+    <row r="205" ht="15.75" customHeight="1"/>
+    <row r="206" ht="15.75" customHeight="1"/>
+    <row r="207" ht="15.75" customHeight="1"/>
+    <row r="208" ht="15.75" customHeight="1"/>
+    <row r="209" ht="15.75" customHeight="1"/>
+    <row r="210" ht="15.75" customHeight="1"/>
+    <row r="211" ht="15.75" customHeight="1"/>
+    <row r="212" ht="15.75" customHeight="1"/>
+    <row r="213" ht="15.75" customHeight="1"/>
+    <row r="214" ht="15.75" customHeight="1"/>
+    <row r="215" ht="15.75" customHeight="1"/>
+    <row r="216" ht="15.75" customHeight="1"/>
+    <row r="217" ht="15.75" customHeight="1"/>
+    <row r="218" ht="15.75" customHeight="1"/>
+    <row r="219" ht="15.75" customHeight="1"/>
+    <row r="220" ht="15.75" customHeight="1"/>
+    <row r="221" ht="15.75" customHeight="1"/>
+    <row r="222" ht="15.75" customHeight="1"/>
+    <row r="223" ht="15.75" customHeight="1"/>
+    <row r="224" ht="15.75" customHeight="1"/>
+    <row r="225" ht="15.75" customHeight="1"/>
+    <row r="226" ht="15.75" customHeight="1"/>
+    <row r="227" ht="15.75" customHeight="1"/>
+    <row r="228" ht="15.75" customHeight="1"/>
+    <row r="229" ht="15.75" customHeight="1"/>
+    <row r="230" ht="15.75" customHeight="1"/>
+    <row r="231" ht="15.75" customHeight="1"/>
+    <row r="232" ht="15.75" customHeight="1"/>
+    <row r="233" ht="15.75" customHeight="1"/>
+    <row r="234" ht="15.75" customHeight="1"/>
+    <row r="235" ht="15.75" customHeight="1"/>
+    <row r="236" ht="15.75" customHeight="1"/>
+    <row r="237" ht="15.75" customHeight="1"/>
+    <row r="238" ht="15.75" customHeight="1"/>
+    <row r="239" ht="15.75" customHeight="1"/>
+    <row r="240" ht="15.75" customHeight="1"/>
+    <row r="241" ht="15.75" customHeight="1"/>
+    <row r="242" ht="15.75" customHeight="1"/>
+    <row r="243" ht="15.75" customHeight="1"/>
+    <row r="244" ht="15.75" customHeight="1"/>
+    <row r="245" ht="15.75" customHeight="1"/>
+    <row r="246" ht="15.75" customHeight="1"/>
+    <row r="247" ht="15.75" customHeight="1"/>
+    <row r="248" ht="15.75" customHeight="1"/>
+    <row r="249" ht="15.75" customHeight="1"/>
+    <row r="250" ht="15.75" customHeight="1"/>
+    <row r="251" ht="15.75" customHeight="1"/>
+    <row r="252" ht="15.75" customHeight="1"/>
+    <row r="253" ht="15.75" customHeight="1"/>
+    <row r="254" ht="15.75" customHeight="1"/>
+    <row r="255" ht="15.75" customHeight="1"/>
+    <row r="256" ht="15.75" customHeight="1"/>
+    <row r="257" ht="15.75" customHeight="1"/>
+    <row r="258" ht="15.75" customHeight="1"/>
+    <row r="259" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1"/>
+    <row r="261" ht="15.75" customHeight="1"/>
+    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="264" ht="15.75" customHeight="1"/>
+    <row r="265" ht="15.75" customHeight="1"/>
+    <row r="266" ht="15.75" customHeight="1"/>
+    <row r="267" ht="15.75" customHeight="1"/>
+    <row r="268" ht="15.75" customHeight="1"/>
+    <row r="269" ht="15.75" customHeight="1"/>
+    <row r="270" ht="15.75" customHeight="1"/>
+    <row r="271" ht="15.75" customHeight="1"/>
+    <row r="272" ht="15.75" customHeight="1"/>
+    <row r="273" ht="15.75" customHeight="1"/>
+    <row r="274" ht="15.75" customHeight="1"/>
+    <row r="275" ht="15.75" customHeight="1"/>
+    <row r="276" ht="15.75" customHeight="1"/>
+    <row r="277" ht="15.75" customHeight="1"/>
+    <row r="278" ht="15.75" customHeight="1"/>
+    <row r="279" ht="15.75" customHeight="1"/>
+    <row r="280" ht="15.75" customHeight="1"/>
+    <row r="281" ht="15.75" customHeight="1"/>
+    <row r="282" ht="15.75" customHeight="1"/>
+    <row r="283" ht="15.75" customHeight="1"/>
+    <row r="284" ht="15.75" customHeight="1"/>
+    <row r="285" ht="15.75" customHeight="1"/>
+    <row r="286" ht="15.75" customHeight="1"/>
+    <row r="287" ht="15.75" customHeight="1"/>
+    <row r="288" ht="15.75" customHeight="1"/>
+    <row r="289" ht="15.75" customHeight="1"/>
+    <row r="290" ht="15.75" customHeight="1"/>
+    <row r="291" ht="15.75" customHeight="1"/>
+    <row r="292" ht="15.75" customHeight="1"/>
+    <row r="293" ht="15.75" customHeight="1"/>
+    <row r="294" ht="15.75" customHeight="1"/>
+    <row r="295" ht="15.75" customHeight="1"/>
+    <row r="296" ht="15.75" customHeight="1"/>
+    <row r="297" ht="15.75" customHeight="1"/>
+    <row r="298" ht="15.75" customHeight="1"/>
+    <row r="299" ht="15.75" customHeight="1"/>
+    <row r="300" ht="15.75" customHeight="1"/>
+    <row r="301" ht="15.75" customHeight="1"/>
+    <row r="302" ht="15.75" customHeight="1"/>
+    <row r="303" ht="15.75" customHeight="1"/>
+    <row r="304" ht="15.75" customHeight="1"/>
+    <row r="305" ht="15.75" customHeight="1"/>
+    <row r="306" ht="15.75" customHeight="1"/>
+    <row r="307" ht="15.75" customHeight="1"/>
+    <row r="308" ht="15.75" customHeight="1"/>
+    <row r="309" ht="15.75" customHeight="1"/>
+    <row r="310" ht="15.75" customHeight="1"/>
+    <row r="311" ht="15.75" customHeight="1"/>
+    <row r="312" ht="15.75" customHeight="1"/>
+    <row r="313" ht="15.75" customHeight="1"/>
+    <row r="314" ht="15.75" customHeight="1"/>
+    <row r="315" ht="15.75" customHeight="1"/>
+    <row r="316" ht="15.75" customHeight="1"/>
+    <row r="317" ht="15.75" customHeight="1"/>
+    <row r="318" ht="15.75" customHeight="1"/>
+    <row r="319" ht="15.75" customHeight="1"/>
+    <row r="320" ht="15.75" customHeight="1"/>
+    <row r="321" ht="15.75" customHeight="1"/>
+    <row r="322" ht="15.75" customHeight="1"/>
+    <row r="323" ht="15.75" customHeight="1"/>
+    <row r="324" ht="15.75" customHeight="1"/>
+    <row r="325" ht="15.75" customHeight="1"/>
+    <row r="326" ht="15.75" customHeight="1"/>
+    <row r="327" ht="15.75" customHeight="1"/>
+    <row r="328" ht="15.75" customHeight="1"/>
+    <row r="329" ht="15.75" customHeight="1"/>
+    <row r="330" ht="15.75" customHeight="1"/>
+    <row r="331" ht="15.75" customHeight="1"/>
+    <row r="332" ht="15.75" customHeight="1"/>
+    <row r="333" ht="15.75" customHeight="1"/>
+    <row r="334" ht="15.75" customHeight="1"/>
+    <row r="335" ht="15.75" customHeight="1"/>
+    <row r="336" ht="15.75" customHeight="1"/>
+    <row r="337" ht="15.75" customHeight="1"/>
+    <row r="338" ht="15.75" customHeight="1"/>
+    <row r="339" ht="15.75" customHeight="1"/>
+    <row r="340" ht="15.75" customHeight="1"/>
+    <row r="341" ht="15.75" customHeight="1"/>
+    <row r="342" ht="15.75" customHeight="1"/>
+    <row r="343" ht="15.75" customHeight="1"/>
+    <row r="344" ht="15.75" customHeight="1"/>
+    <row r="345" ht="15.75" customHeight="1"/>
+    <row r="346" ht="15.75" customHeight="1"/>
+    <row r="347" ht="15.75" customHeight="1"/>
+    <row r="348" ht="15.75" customHeight="1"/>
+    <row r="349" ht="15.75" customHeight="1"/>
+    <row r="350" ht="15.75" customHeight="1"/>
+    <row r="351" ht="15.75" customHeight="1"/>
+    <row r="352" ht="15.75" customHeight="1"/>
+    <row r="353" ht="15.75" customHeight="1"/>
+    <row r="354" ht="15.75" customHeight="1"/>
+    <row r="355" ht="15.75" customHeight="1"/>
+    <row r="356" ht="15.75" customHeight="1"/>
+    <row r="357" ht="15.75" customHeight="1"/>
+    <row r="358" ht="15.75" customHeight="1"/>
+    <row r="359" ht="15.75" customHeight="1"/>
+    <row r="360" ht="15.75" customHeight="1"/>
+    <row r="361" ht="15.75" customHeight="1"/>
+    <row r="362" ht="15.75" customHeight="1"/>
+    <row r="363" ht="15.75" customHeight="1"/>
+    <row r="364" ht="15.75" customHeight="1"/>
+    <row r="365" ht="15.75" customHeight="1"/>
+    <row r="366" ht="15.75" customHeight="1"/>
+    <row r="367" ht="15.75" customHeight="1"/>
+    <row r="368" ht="15.75" customHeight="1"/>
+    <row r="369" ht="15.75" customHeight="1"/>
+    <row r="370" ht="15.75" customHeight="1"/>
+    <row r="371" ht="15.75" customHeight="1"/>
+    <row r="372" ht="15.75" customHeight="1"/>
+    <row r="373" ht="15.75" customHeight="1"/>
+    <row r="374" ht="15.75" customHeight="1"/>
+    <row r="375" ht="15.75" customHeight="1"/>
+    <row r="376" ht="15.75" customHeight="1"/>
+    <row r="377" ht="15.75" customHeight="1"/>
+    <row r="378" ht="15.75" customHeight="1"/>
+    <row r="379" ht="15.75" customHeight="1"/>
+    <row r="380" ht="15.75" customHeight="1"/>
+    <row r="381" ht="15.75" customHeight="1"/>
+    <row r="382" ht="15.75" customHeight="1"/>
+    <row r="383" ht="15.75" customHeight="1"/>
+    <row r="384" ht="15.75" customHeight="1"/>
+    <row r="385" ht="15.75" customHeight="1"/>
+    <row r="386" ht="15.75" customHeight="1"/>
+    <row r="387" ht="15.75" customHeight="1"/>
+    <row r="388" ht="15.75" customHeight="1"/>
+    <row r="389" ht="15.75" customHeight="1"/>
+    <row r="390" ht="15.75" customHeight="1"/>
+    <row r="391" ht="15.75" customHeight="1"/>
+    <row r="392" ht="15.75" customHeight="1"/>
+    <row r="393" ht="15.75" customHeight="1"/>
+    <row r="394" ht="15.75" customHeight="1"/>
+    <row r="395" ht="15.75" customHeight="1"/>
+    <row r="396" ht="15.75" customHeight="1"/>
+    <row r="397" ht="15.75" customHeight="1"/>
+    <row r="398" ht="15.75" customHeight="1"/>
+    <row r="399" ht="15.75" customHeight="1"/>
+    <row r="400" ht="15.75" customHeight="1"/>
+    <row r="401" ht="15.75" customHeight="1"/>
+    <row r="402" ht="15.75" customHeight="1"/>
+    <row r="403" ht="15.75" customHeight="1"/>
+    <row r="404" ht="15.75" customHeight="1"/>
+    <row r="405" ht="15.75" customHeight="1"/>
+    <row r="406" ht="15.75" customHeight="1"/>
+    <row r="407" ht="15.75" customHeight="1"/>
+    <row r="408" ht="15.75" customHeight="1"/>
+    <row r="409" ht="15.75" customHeight="1"/>
+    <row r="410" ht="15.75" customHeight="1"/>
+    <row r="411" ht="15.75" customHeight="1"/>
+    <row r="412" ht="15.75" customHeight="1"/>
+    <row r="413" ht="15.75" customHeight="1"/>
+    <row r="414" ht="15.75" customHeight="1"/>
+    <row r="415" ht="15.75" customHeight="1"/>
+    <row r="416" ht="15.75" customHeight="1"/>
+    <row r="417" ht="15.75" customHeight="1"/>
+    <row r="418" ht="15.75" customHeight="1"/>
+    <row r="419" ht="15.75" customHeight="1"/>
+    <row r="420" ht="15.75" customHeight="1"/>
+    <row r="421" ht="15.75" customHeight="1"/>
+    <row r="422" ht="15.75" customHeight="1"/>
+    <row r="423" ht="15.75" customHeight="1"/>
+    <row r="424" ht="15.75" customHeight="1"/>
+    <row r="425" ht="15.75" customHeight="1"/>
+    <row r="426" ht="15.75" customHeight="1"/>
+    <row r="427" ht="15.75" customHeight="1"/>
+    <row r="428" ht="15.75" customHeight="1"/>
+    <row r="429" ht="15.75" customHeight="1"/>
+    <row r="430" ht="15.75" customHeight="1"/>
+    <row r="431" ht="15.75" customHeight="1"/>
+    <row r="432" ht="15.75" customHeight="1"/>
+    <row r="433" ht="15.75" customHeight="1"/>
+    <row r="434" ht="15.75" customHeight="1"/>
+    <row r="435" ht="15.75" customHeight="1"/>
+    <row r="436" ht="15.75" customHeight="1"/>
+    <row r="437" ht="15.75" customHeight="1"/>
+    <row r="438" ht="15.75" customHeight="1"/>
+    <row r="439" ht="15.75" customHeight="1"/>
+    <row r="440" ht="15.75" customHeight="1"/>
+    <row r="441" ht="15.75" customHeight="1"/>
+    <row r="442" ht="15.75" customHeight="1"/>
+    <row r="443" ht="15.75" customHeight="1"/>
+    <row r="444" ht="15.75" customHeight="1"/>
+    <row r="445" ht="15.75" customHeight="1"/>
+    <row r="446" ht="15.75" customHeight="1"/>
+    <row r="447" ht="15.75" customHeight="1"/>
+    <row r="448" ht="15.75" customHeight="1"/>
+    <row r="449" ht="15.75" customHeight="1"/>
+    <row r="450" ht="15.75" customHeight="1"/>
+    <row r="451" ht="15.75" customHeight="1"/>
+    <row r="452" ht="15.75" customHeight="1"/>
+    <row r="453" ht="15.75" customHeight="1"/>
+    <row r="454" ht="15.75" customHeight="1"/>
+    <row r="455" ht="15.75" customHeight="1"/>
+    <row r="456" ht="15.75" customHeight="1"/>
+    <row r="457" ht="15.75" customHeight="1"/>
+    <row r="458" ht="15.75" customHeight="1"/>
+    <row r="459" ht="15.75" customHeight="1"/>
+    <row r="460" ht="15.75" customHeight="1"/>
+    <row r="461" ht="15.75" customHeight="1"/>
+    <row r="462" ht="15.75" customHeight="1"/>
+    <row r="463" ht="15.75" customHeight="1"/>
+    <row r="464" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>